<commit_message>
Pie chart - Hgld + Nrge
</commit_message>
<xml_diff>
--- a/Data_R_MSB_210/NACE_kake_2021.xlsx
+++ b/Data_R_MSB_210/NACE_kake_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindreespedal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindreespedal/Documents/HVL /Vaar_2023/The_thesis/Data_R_MSB_210/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A01E6F4-5E93-E442-B54A-3BCA934AB8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFF71CE-521E-B64F-8D56-F26C0ECB5CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14020" yWindow="920" windowWidth="14400" windowHeight="16520" xr2:uid="{C9488A84-6FF8-504C-A99C-293E6464ADF8}"/>
   </bookViews>
@@ -50,70 +50,70 @@
     <t>Haugalandet</t>
   </si>
   <si>
-    <t>A - Jordbruk, skogbruk og fiske (01-03)</t>
-  </si>
-  <si>
-    <t>B - Bergverkdrift og utvinning (05-09)</t>
-  </si>
-  <si>
-    <t>C - Industri (10-33)</t>
-  </si>
-  <si>
-    <t>D - Elektrisitets-, gass-, damp- og varmtvannsforsyning (35)</t>
-  </si>
-  <si>
-    <t>E - Vannforsyning, avløps- og renovasjonsvirksomhet (36-39)</t>
-  </si>
-  <si>
-    <t>F - Bygge- og anleggsvirksomhet (41-43)</t>
-  </si>
-  <si>
-    <t>G - Varehandel, reparasjon av motorvogner (45-47)</t>
-  </si>
-  <si>
-    <t>H - Transport og lagring (49-53)</t>
-  </si>
-  <si>
-    <t>I - Overnattings- og serveringsvirksomhet (55-56)</t>
-  </si>
-  <si>
-    <t>J - Informasjon og kommunikasjon (58-63)</t>
-  </si>
-  <si>
-    <t>K - Finansierings- og forsikringsvirksomhet (64-66)</t>
-  </si>
-  <si>
-    <t>L - Omsetning og drift av fast eiendom (68)</t>
-  </si>
-  <si>
-    <t>M - Faglig, vitenskapelig og teknisk tjenesteyting (69-75)</t>
-  </si>
-  <si>
-    <t>N - Forretningsmessig tjenesteyting (77-82)</t>
-  </si>
-  <si>
-    <t>O - Offentlig administrasjon og forsvar, og trygdeordninger underlagt offentlig forvaltning (84)</t>
-  </si>
-  <si>
-    <t>P - Undervisning (85)</t>
-  </si>
-  <si>
-    <t>Q - Helse- og sosialtjenester (86-88)</t>
-  </si>
-  <si>
-    <t>R - Kulturell virksomhet, underholdning og fritidsaktiviteter (90-93)</t>
-  </si>
-  <si>
-    <t>S - Annen tjenesteyting (94-96)</t>
-  </si>
-  <si>
-    <t>T - Lønnet arbeid i private husholdninger (97)</t>
-  </si>
-  <si>
-    <t>U - Internasjonale organisasjoner og organer (99)</t>
-  </si>
-  <si>
     <t>Norge</t>
+  </si>
+  <si>
+    <t>A - (01-03)</t>
+  </si>
+  <si>
+    <t>B - (05-09)</t>
+  </si>
+  <si>
+    <t>C - (10-33)</t>
+  </si>
+  <si>
+    <t>D - (35)</t>
+  </si>
+  <si>
+    <t>E - (36-39)</t>
+  </si>
+  <si>
+    <t>F - (41-43)</t>
+  </si>
+  <si>
+    <t>G - (45-47)</t>
+  </si>
+  <si>
+    <t>H - (49-53)</t>
+  </si>
+  <si>
+    <t>I - (55-56)</t>
+  </si>
+  <si>
+    <t>J - (58-63)</t>
+  </si>
+  <si>
+    <t>K - (64-66)</t>
+  </si>
+  <si>
+    <t>L - (68)</t>
+  </si>
+  <si>
+    <t>M - (69-75)</t>
+  </si>
+  <si>
+    <t>N - (77-82)</t>
+  </si>
+  <si>
+    <t>O - (84)</t>
+  </si>
+  <si>
+    <t>P - (85)</t>
+  </si>
+  <si>
+    <t>Q - (86-88)</t>
+  </si>
+  <si>
+    <t>R - (90-93)</t>
+  </si>
+  <si>
+    <t>S - (94-96)</t>
+  </si>
+  <si>
+    <t>T - (97)</t>
+  </si>
+  <si>
+    <t>U - (99)</t>
   </si>
 </sst>
 </file>
@@ -477,10 +477,13 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="45" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -498,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>3.04</v>
@@ -509,7 +512,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>3.16</v>
@@ -520,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>12.68</v>
@@ -531,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0.95</v>
@@ -542,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>0.71</v>
@@ -553,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>9.35</v>
@@ -564,7 +567,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>12.39</v>
@@ -575,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>5.95</v>
@@ -586,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>2.72</v>
@@ -597,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>2.15</v>
@@ -608,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>0.51</v>
@@ -619,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>0.64</v>
@@ -630,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>3.37</v>
@@ -641,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>4.57</v>
@@ -652,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>4.2300000000000004</v>
@@ -663,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>8.31</v>
@@ -674,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>22.5</v>
@@ -685,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>1.1499999999999999</v>
@@ -696,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>1.6</v>
@@ -707,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>0.01</v>
@@ -718,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -726,10 +729,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>2.3199999999999998</v>
@@ -737,10 +740,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>2.17</v>
@@ -748,10 +751,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>7.65</v>
@@ -759,10 +762,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>0.61</v>
@@ -770,10 +773,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>0.61</v>
@@ -781,10 +784,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>8.66</v>
@@ -792,10 +795,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29">
         <v>12.81</v>
@@ -803,10 +806,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C30">
         <v>4.7300000000000004</v>
@@ -814,10 +817,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31">
         <v>3.47</v>
@@ -825,10 +828,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>3.95</v>
@@ -836,10 +839,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33">
         <v>1.76</v>
@@ -847,10 +850,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34">
         <v>1.01</v>
@@ -858,10 +861,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C35">
         <v>5.59</v>
@@ -869,10 +872,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36">
         <v>4.92</v>
@@ -880,10 +883,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>6.37</v>
@@ -891,10 +894,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C38">
         <v>8.36</v>
@@ -902,10 +905,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C39">
         <v>20.89</v>
@@ -913,10 +916,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>2.06</v>
@@ -924,10 +927,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C41">
         <v>2.02</v>
@@ -935,10 +938,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C42">
         <v>0.03</v>
@@ -946,10 +949,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
         <v>25</v>
-      </c>
-      <c r="B43" t="s">
-        <v>24</v>
       </c>
       <c r="C43">
         <v>0.01</v>

</xml_diff>